<commit_message>
New graph for interannual lipid fluctuation and improved other graphs
</commit_message>
<xml_diff>
--- a/krillINFO_months.xlsx
+++ b/krillINFO_months.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6bc14b3081350469/Old/placement/alfred-wegener/Bettina Meyer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_A4407568C3574AFC12484884CAAB988C2309E9E0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2C47D95-F5E4-44F4-993B-D49D4E0A8B35}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_D3447670C3574AFC124848038AACBA62230959F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4194D8A6-4BA9-41D2-BAC8-CB4445F87FFC}"/>
   <bookViews>
-    <workbookView xWindow="12090" yWindow="-14490" windowWidth="21600" windowHeight="12405" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="master" sheetId="1" r:id="rId1"/>
-    <sheet name="JAS" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">master!$A$1:$D$133</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$133</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="32">
   <si>
     <t>yr</t>
   </si>
@@ -51,6 +51,39 @@
     <t>sdLipids</t>
   </si>
   <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
     <t>January</t>
   </si>
   <si>
@@ -87,10 +120,10 @@
     <t>December</t>
   </si>
   <si>
+    <t>julLips</t>
+  </si>
+  <si>
     <t>augLips</t>
-  </si>
-  <si>
-    <t>julLips</t>
   </si>
   <si>
     <t>sepLips</t>
@@ -137,7 +170,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,25 +509,25 @@
       </c>
     </row>
     <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="1">
-        <v>2011</v>
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D2" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D2" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
-        <v>2011</v>
-      </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>10.372826086956522</v>
@@ -504,11 +537,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
-        <v>2011</v>
+      <c r="A4" t="s">
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>16.940639999999998</v>
@@ -518,11 +551,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="1">
-        <v>2011</v>
+      <c r="A5" t="s">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>24.948600000000003</v>
@@ -532,11 +565,11 @@
       </c>
     </row>
     <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
-        <v>2011</v>
+      <c r="A6" t="s">
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>18.646041666666665</v>
@@ -546,11 +579,11 @@
       </c>
     </row>
     <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="1">
-        <v>2011</v>
+      <c r="A7" t="s">
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C7">
         <v>3.028833333333333</v>
@@ -560,11 +593,11 @@
       </c>
     </row>
     <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="1">
-        <v>2011</v>
+      <c r="A8" t="s">
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>6.4621649484536086</v>
@@ -574,11 +607,11 @@
       </c>
     </row>
     <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="1">
-        <v>2011</v>
+      <c r="A9" t="s">
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>17.041290322580643</v>
@@ -588,11 +621,11 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="1">
-        <v>2011</v>
+      <c r="A10" t="s">
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C10">
         <v>5.0483333333333338</v>
@@ -602,11 +635,11 @@
       </c>
     </row>
     <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="1">
-        <v>2011</v>
+      <c r="A11" t="s">
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C11" t="e">
         <v>#N/A</v>
@@ -616,11 +649,11 @@
       </c>
     </row>
     <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="1">
-        <v>2011</v>
+      <c r="A12" t="s">
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C12" t="e">
         <v>#N/A</v>
@@ -630,11 +663,11 @@
       </c>
     </row>
     <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="1">
-        <v>2011</v>
+      <c r="A13" t="s">
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C13">
         <v>15.173152173913044</v>
@@ -644,11 +677,11 @@
       </c>
     </row>
     <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="1">
-        <v>2012</v>
+      <c r="A14" t="s">
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>12.594895833333332</v>
@@ -658,11 +691,11 @@
       </c>
     </row>
     <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="1">
-        <v>2012</v>
+      <c r="A15" t="s">
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>18.172767857142855</v>
@@ -672,11 +705,11 @@
       </c>
     </row>
     <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="1">
-        <v>2012</v>
+      <c r="A16" t="s">
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>12.096323529411764</v>
@@ -686,11 +719,11 @@
       </c>
     </row>
     <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="1">
-        <v>2012</v>
+      <c r="A17" t="s">
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>14.516532258064515</v>
@@ -700,11 +733,11 @@
       </c>
     </row>
     <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="1">
-        <v>2012</v>
+      <c r="A18" t="s">
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>10.017916666666666</v>
@@ -714,11 +747,11 @@
       </c>
     </row>
     <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="1">
-        <v>2012</v>
+      <c r="A19" t="s">
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C19">
         <v>3.7610377358490568</v>
@@ -728,11 +761,11 @@
       </c>
     </row>
     <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="1">
-        <v>2012</v>
+      <c r="A20" t="s">
+        <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>1.400532786885246</v>
@@ -742,39 +775,39 @@
       </c>
     </row>
     <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="1">
-        <v>2012</v>
+      <c r="A21" t="s">
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="C21" t="e">
+        <v>#N/A</v>
       </c>
       <c r="D21" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="1">
-        <v>2012</v>
+      <c r="A22" t="s">
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="C22" t="e">
+        <v>#N/A</v>
       </c>
       <c r="D22" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="1">
-        <v>2012</v>
+      <c r="A23" t="s">
+        <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C23" t="e">
         <v>#N/A</v>
@@ -784,11 +817,11 @@
       </c>
     </row>
     <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="1">
-        <v>2012</v>
+      <c r="A24" t="s">
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C24" t="e">
         <v>#N/A</v>
@@ -798,25 +831,25 @@
       </c>
     </row>
     <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="1">
-        <v>2012</v>
+      <c r="A25" t="s">
+        <v>5</v>
       </c>
       <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D25" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
         <v>15</v>
-      </c>
-      <c r="C25" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D25" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="1">
-        <v>2013</v>
-      </c>
-      <c r="B26" t="s">
-        <v>4</v>
       </c>
       <c r="C26">
         <v>4.2663815789473682</v>
@@ -826,11 +859,11 @@
       </c>
     </row>
     <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="1">
-        <v>2013</v>
+      <c r="A27" t="s">
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C27">
         <v>9.4629545454545454</v>
@@ -840,11 +873,11 @@
       </c>
     </row>
     <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="1">
-        <v>2013</v>
+      <c r="A28" t="s">
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C28">
         <v>7.7210211267605633</v>
@@ -854,11 +887,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="1">
-        <v>2013</v>
+      <c r="A29" t="s">
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C29">
         <v>7.4309829059829058</v>
@@ -868,11 +901,11 @@
       </c>
     </row>
     <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="1">
-        <v>2013</v>
+      <c r="A30" t="s">
+        <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C30">
         <v>5.7281976744186043</v>
@@ -882,11 +915,11 @@
       </c>
     </row>
     <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="1">
-        <v>2013</v>
+      <c r="A31" t="s">
+        <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C31">
         <v>6.8081363636363639</v>
@@ -896,11 +929,11 @@
       </c>
     </row>
     <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="1">
-        <v>2013</v>
+      <c r="A32" t="s">
+        <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C32">
         <v>5.7643023255813954</v>
@@ -910,11 +943,11 @@
       </c>
     </row>
     <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="1">
-        <v>2013</v>
+      <c r="A33" t="s">
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C33">
         <v>5.6309756097560975</v>
@@ -924,53 +957,53 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A34" s="1">
-        <v>2013</v>
+      <c r="A34" t="s">
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="C34" t="e">
+        <v>#N/A</v>
       </c>
       <c r="D34" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="1">
-        <v>2013</v>
+      <c r="A35" t="s">
+        <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="C35" t="e">
+        <v>#N/A</v>
       </c>
       <c r="D35" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="1">
-        <v>2013</v>
+      <c r="A36" t="s">
+        <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="C36" t="e">
+        <v>#N/A</v>
       </c>
       <c r="D36" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="1">
-        <v>2013</v>
+      <c r="A37" t="s">
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C37">
         <v>14.980301204819277</v>
@@ -980,11 +1013,11 @@
       </c>
     </row>
     <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="1">
-        <v>2014</v>
+      <c r="A38" t="s">
+        <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C38">
         <v>7.1452784090909089</v>
@@ -994,11 +1027,11 @@
       </c>
     </row>
     <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="1">
-        <v>2014</v>
+      <c r="A39" t="s">
+        <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C39">
         <v>8.6319018404907979</v>
@@ -1008,11 +1041,11 @@
       </c>
     </row>
     <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="1">
-        <v>2014</v>
+      <c r="A40" t="s">
+        <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C40">
         <v>6.8333921568627449</v>
@@ -1022,11 +1055,11 @@
       </c>
     </row>
     <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="1">
-        <v>2014</v>
+      <c r="A41" t="s">
+        <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C41">
         <v>6.7200571428571427</v>
@@ -1036,11 +1069,11 @@
       </c>
     </row>
     <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="1">
-        <v>2014</v>
+      <c r="A42" t="s">
+        <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C42">
         <v>5.7286224489795918</v>
@@ -1050,11 +1083,11 @@
       </c>
     </row>
     <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="1">
-        <v>2014</v>
+      <c r="A43" t="s">
+        <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C43">
         <v>6.8937499999999998</v>
@@ -1064,11 +1097,11 @@
       </c>
     </row>
     <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="1">
-        <v>2014</v>
+      <c r="A44" t="s">
+        <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C44">
         <v>8.3901538461538454</v>
@@ -1078,11 +1111,11 @@
       </c>
     </row>
     <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="1">
-        <v>2014</v>
+      <c r="A45" t="s">
+        <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C45">
         <v>12.558092105263157</v>
@@ -1092,11 +1125,11 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A46" s="1">
-        <v>2014</v>
+      <c r="A46" t="s">
+        <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C46">
         <v>14.717558333333333</v>
@@ -1106,11 +1139,11 @@
       </c>
     </row>
     <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="1">
-        <v>2014</v>
+      <c r="A47" t="s">
+        <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C47" t="e">
         <v>#N/A</v>
@@ -1120,11 +1153,11 @@
       </c>
     </row>
     <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="1">
-        <v>2014</v>
+      <c r="A48" t="s">
+        <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C48" t="e">
         <v>#N/A</v>
@@ -1134,11 +1167,11 @@
       </c>
     </row>
     <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="1">
-        <v>2014</v>
+      <c r="A49" t="s">
+        <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C49">
         <v>17.136785714285715</v>
@@ -1148,11 +1181,11 @@
       </c>
     </row>
     <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="1">
-        <v>2015</v>
+      <c r="A50" t="s">
+        <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C50">
         <v>10.453719512195123</v>
@@ -1162,11 +1195,11 @@
       </c>
     </row>
     <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="1">
-        <v>2015</v>
+      <c r="A51" t="s">
+        <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C51">
         <v>14.489558448717949</v>
@@ -1176,11 +1209,11 @@
       </c>
     </row>
     <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="1">
-        <v>2015</v>
+      <c r="A52" t="s">
+        <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C52">
         <v>21.254319166666669</v>
@@ -1190,11 +1223,11 @@
       </c>
     </row>
     <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="1">
-        <v>2015</v>
+      <c r="A53" t="s">
+        <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C53">
         <v>16.255012195121953</v>
@@ -1204,11 +1237,11 @@
       </c>
     </row>
     <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="1">
-        <v>2015</v>
+      <c r="A54" t="s">
+        <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C54">
         <v>22.527334999999997</v>
@@ -1218,11 +1251,11 @@
       </c>
     </row>
     <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="1">
-        <v>2015</v>
+      <c r="A55" t="s">
+        <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C55">
         <v>11.609368932038835</v>
@@ -1232,11 +1265,11 @@
       </c>
     </row>
     <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="1">
-        <v>2015</v>
+      <c r="A56" t="s">
+        <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C56">
         <v>9.2674566473988431</v>
@@ -1246,11 +1279,11 @@
       </c>
     </row>
     <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="1">
-        <v>2015</v>
+      <c r="A57" t="s">
+        <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C57">
         <v>11.038570620938627</v>
@@ -1260,11 +1293,11 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A58" s="1">
-        <v>2015</v>
+      <c r="A58" t="s">
+        <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C58">
         <v>11.547362475</v>
@@ -1274,11 +1307,11 @@
       </c>
     </row>
     <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="1">
-        <v>2015</v>
+      <c r="A59" t="s">
+        <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C59" t="e">
         <v>#N/A</v>
@@ -1288,11 +1321,11 @@
       </c>
     </row>
     <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="1">
-        <v>2015</v>
+      <c r="A60" t="s">
+        <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C60" t="e">
         <v>#N/A</v>
@@ -1302,11 +1335,11 @@
       </c>
     </row>
     <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="1">
-        <v>2015</v>
+      <c r="A61" t="s">
+        <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C61">
         <v>26.253224481818179</v>
@@ -1316,11 +1349,11 @@
       </c>
     </row>
     <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="1">
-        <v>2016</v>
+      <c r="A62" t="s">
+        <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C62">
         <v>20.292668119760478</v>
@@ -1330,11 +1363,11 @@
       </c>
     </row>
     <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="1">
-        <v>2016</v>
+      <c r="A63" t="s">
+        <v>9</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C63">
         <v>12.432289156626508</v>
@@ -1344,11 +1377,11 @@
       </c>
     </row>
     <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="1">
-        <v>2016</v>
+      <c r="A64" t="s">
+        <v>9</v>
       </c>
       <c r="B64" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C64">
         <v>12.047258064516129</v>
@@ -1358,11 +1391,11 @@
       </c>
     </row>
     <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="1">
-        <v>2016</v>
+      <c r="A65" t="s">
+        <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C65">
         <v>10.083630729885057</v>
@@ -1372,11 +1405,11 @@
       </c>
     </row>
     <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="1">
-        <v>2016</v>
+      <c r="A66" t="s">
+        <v>9</v>
       </c>
       <c r="B66" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C66">
         <v>10.692890804597702</v>
@@ -1386,11 +1419,11 @@
       </c>
     </row>
     <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="1">
-        <v>2016</v>
+      <c r="A67" t="s">
+        <v>9</v>
       </c>
       <c r="B67" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C67">
         <v>5.1509757575757575</v>
@@ -1400,11 +1433,11 @@
       </c>
     </row>
     <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A68" s="1">
-        <v>2016</v>
+      <c r="A68" t="s">
+        <v>9</v>
       </c>
       <c r="B68" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C68">
         <v>7.7638709677419362</v>
@@ -1414,11 +1447,11 @@
       </c>
     </row>
     <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="1">
-        <v>2016</v>
+      <c r="A69" t="s">
+        <v>9</v>
       </c>
       <c r="B69" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C69">
         <v>8.9742483660130716</v>
@@ -1428,11 +1461,11 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A70" s="1">
-        <v>2016</v>
+      <c r="A70" t="s">
+        <v>9</v>
       </c>
       <c r="B70" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C70">
         <v>10.890923076923077</v>
@@ -1442,11 +1475,11 @@
       </c>
     </row>
     <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A71" s="1">
-        <v>2016</v>
+      <c r="A71" t="s">
+        <v>9</v>
       </c>
       <c r="B71" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C71" t="e">
         <v>#N/A</v>
@@ -1456,11 +1489,11 @@
       </c>
     </row>
     <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="1">
-        <v>2016</v>
+      <c r="A72" t="s">
+        <v>9</v>
       </c>
       <c r="B72" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C72" t="e">
         <v>#N/A</v>
@@ -1470,11 +1503,11 @@
       </c>
     </row>
     <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="1">
-        <v>2016</v>
+      <c r="A73" t="s">
+        <v>9</v>
       </c>
       <c r="B73" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C73">
         <v>18.113820464285716</v>
@@ -1484,11 +1517,11 @@
       </c>
     </row>
     <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A74" s="1">
-        <v>2017</v>
+      <c r="A74" t="s">
+        <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C74">
         <v>13.707363157894736</v>
@@ -1498,11 +1531,11 @@
       </c>
     </row>
     <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A75" s="1">
-        <v>2017</v>
+      <c r="A75" t="s">
+        <v>10</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C75">
         <v>13.9955</v>
@@ -1512,11 +1545,11 @@
       </c>
     </row>
     <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="1">
-        <v>2017</v>
+      <c r="A76" t="s">
+        <v>10</v>
       </c>
       <c r="B76" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C76">
         <v>17.684747311827955</v>
@@ -1526,11 +1559,11 @@
       </c>
     </row>
     <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A77" s="1">
-        <v>2017</v>
+      <c r="A77" t="s">
+        <v>10</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C77">
         <v>16.665561497326202</v>
@@ -1540,11 +1573,11 @@
       </c>
     </row>
     <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A78" s="1">
-        <v>2017</v>
+      <c r="A78" t="s">
+        <v>10</v>
       </c>
       <c r="B78" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C78">
         <v>17.990380952380953</v>
@@ -1554,11 +1587,11 @@
       </c>
     </row>
     <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A79" s="1">
-        <v>2017</v>
+      <c r="A79" t="s">
+        <v>10</v>
       </c>
       <c r="B79" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C79">
         <v>10.339846153846153</v>
@@ -1568,11 +1601,11 @@
       </c>
     </row>
     <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A80" s="1">
-        <v>2017</v>
+      <c r="A80" t="s">
+        <v>10</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C80">
         <v>9.9817204301075257</v>
@@ -1582,11 +1615,11 @@
       </c>
     </row>
     <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A81" s="1">
-        <v>2017</v>
+      <c r="A81" t="s">
+        <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C81">
         <v>2.986470588235294</v>
@@ -1596,11 +1629,11 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A82" s="1">
-        <v>2017</v>
+      <c r="A82" t="s">
+        <v>10</v>
       </c>
       <c r="B82" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C82" t="e">
         <v>#N/A</v>
@@ -1610,11 +1643,11 @@
       </c>
     </row>
     <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A83" s="1">
-        <v>2017</v>
+      <c r="A83" t="s">
+        <v>10</v>
       </c>
       <c r="B83" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C83" t="e">
         <v>#N/A</v>
@@ -1624,11 +1657,11 @@
       </c>
     </row>
     <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A84" s="1">
-        <v>2017</v>
+      <c r="A84" t="s">
+        <v>10</v>
       </c>
       <c r="B84" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C84" t="e">
         <v>#N/A</v>
@@ -1638,11 +1671,11 @@
       </c>
     </row>
     <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A85" s="1">
-        <v>2017</v>
+      <c r="A85" t="s">
+        <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C85">
         <v>13.429071428571428</v>
@@ -1652,11 +1685,11 @@
       </c>
     </row>
     <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A86" s="1">
-        <v>2018</v>
+      <c r="A86" t="s">
+        <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C86">
         <v>11.453947368421053</v>
@@ -1666,11 +1699,11 @@
       </c>
     </row>
     <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A87" s="1">
-        <v>2018</v>
+      <c r="A87" t="s">
+        <v>11</v>
       </c>
       <c r="B87" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C87">
         <v>8.2372312500000007</v>
@@ -1680,11 +1713,11 @@
       </c>
     </row>
     <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A88" s="1">
-        <v>2018</v>
+      <c r="A88" t="s">
+        <v>11</v>
       </c>
       <c r="B88" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C88">
         <v>14.905844155844155</v>
@@ -1694,11 +1727,11 @@
       </c>
     </row>
     <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A89" s="1">
-        <v>2018</v>
+      <c r="A89" t="s">
+        <v>11</v>
       </c>
       <c r="B89" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C89">
         <v>17.930679144385024</v>
@@ -1708,11 +1741,11 @@
       </c>
     </row>
     <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A90" s="1">
-        <v>2018</v>
+      <c r="A90" t="s">
+        <v>11</v>
       </c>
       <c r="B90" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C90">
         <v>15.42543875598086</v>
@@ -1722,11 +1755,11 @@
       </c>
     </row>
     <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A91" s="1">
-        <v>2018</v>
+      <c r="A91" t="s">
+        <v>11</v>
       </c>
       <c r="B91" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C91">
         <v>16.534170905294477</v>
@@ -1736,11 +1769,11 @@
       </c>
     </row>
     <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A92" s="1">
-        <v>2018</v>
+      <c r="A92" t="s">
+        <v>11</v>
       </c>
       <c r="B92" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C92">
         <v>12.320102225206107</v>
@@ -1750,11 +1783,11 @@
       </c>
     </row>
     <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A93" s="1">
-        <v>2018</v>
+      <c r="A93" t="s">
+        <v>11</v>
       </c>
       <c r="B93" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C93">
         <v>7.3007031914624276</v>
@@ -1764,11 +1797,11 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A94" s="1">
-        <v>2018</v>
+      <c r="A94" t="s">
+        <v>11</v>
       </c>
       <c r="B94" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C94">
         <v>9.5609655172413781</v>
@@ -1778,11 +1811,11 @@
       </c>
     </row>
     <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A95" s="1">
-        <v>2018</v>
+      <c r="A95" t="s">
+        <v>11</v>
       </c>
       <c r="B95" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C95">
         <v>14.220526315789474</v>
@@ -1792,11 +1825,11 @@
       </c>
     </row>
     <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A96" s="1">
-        <v>2018</v>
+      <c r="A96" t="s">
+        <v>11</v>
       </c>
       <c r="B96" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C96" t="e">
         <v>#N/A</v>
@@ -1806,11 +1839,11 @@
       </c>
     </row>
     <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A97" s="1">
-        <v>2018</v>
+      <c r="A97" t="s">
+        <v>11</v>
       </c>
       <c r="B97" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C97">
         <v>36.187363636363635</v>
@@ -1820,11 +1853,11 @@
       </c>
     </row>
     <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A98" s="1">
-        <v>2019</v>
+      <c r="A98" t="s">
+        <v>12</v>
       </c>
       <c r="B98" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C98">
         <v>33.001769911504425</v>
@@ -1834,11 +1867,11 @@
       </c>
     </row>
     <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A99" s="1">
-        <v>2019</v>
+      <c r="A99" t="s">
+        <v>12</v>
       </c>
       <c r="B99" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C99">
         <v>30.670104166666665</v>
@@ -1848,11 +1881,11 @@
       </c>
     </row>
     <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A100" s="1">
-        <v>2019</v>
+      <c r="A100" t="s">
+        <v>12</v>
       </c>
       <c r="B100" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C100">
         <v>29.390303030303031</v>
@@ -1862,11 +1895,11 @@
       </c>
     </row>
     <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A101" s="1">
-        <v>2019</v>
+      <c r="A101" t="s">
+        <v>12</v>
       </c>
       <c r="B101" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C101">
         <v>32.478437499999998</v>
@@ -1876,11 +1909,11 @@
       </c>
     </row>
     <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A102" s="1">
-        <v>2019</v>
+      <c r="A102" t="s">
+        <v>12</v>
       </c>
       <c r="B102" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C102">
         <v>30.193103448275863</v>
@@ -1890,11 +1923,11 @@
       </c>
     </row>
     <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A103" s="1">
-        <v>2019</v>
+      <c r="A103" t="s">
+        <v>12</v>
       </c>
       <c r="B103" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C103">
         <v>29.715583333333331</v>
@@ -1904,11 +1937,11 @@
       </c>
     </row>
     <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A104" s="1">
-        <v>2019</v>
+      <c r="A104" t="s">
+        <v>12</v>
       </c>
       <c r="B104" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C104">
         <v>24.190280373831776</v>
@@ -1918,11 +1951,11 @@
       </c>
     </row>
     <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A105" s="1">
-        <v>2019</v>
+      <c r="A105" t="s">
+        <v>12</v>
       </c>
       <c r="B105" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C105">
         <v>17.456099290780141</v>
@@ -1932,11 +1965,11 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A106" s="1">
-        <v>2019</v>
+      <c r="A106" t="s">
+        <v>12</v>
       </c>
       <c r="B106" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C106">
         <v>32.15717647058824</v>
@@ -1946,11 +1979,11 @@
       </c>
     </row>
     <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A107" s="1">
-        <v>2019</v>
+      <c r="A107" t="s">
+        <v>12</v>
       </c>
       <c r="B107" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C107" t="e">
         <v>#N/A</v>
@@ -1960,11 +1993,11 @@
       </c>
     </row>
     <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A108" s="1">
-        <v>2019</v>
+      <c r="A108" t="s">
+        <v>12</v>
       </c>
       <c r="B108" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C108" t="e">
         <v>#N/A</v>
@@ -1974,11 +2007,11 @@
       </c>
     </row>
     <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A109" s="1">
-        <v>2019</v>
+      <c r="A109" t="s">
+        <v>12</v>
       </c>
       <c r="B109" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C109">
         <v>33.812077646000006</v>
@@ -1988,11 +2021,11 @@
       </c>
     </row>
     <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A110" s="1">
-        <v>2020</v>
+      <c r="A110" t="s">
+        <v>13</v>
       </c>
       <c r="B110" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C110">
         <v>30.212147337094596</v>
@@ -2002,11 +2035,11 @@
       </c>
     </row>
     <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A111" s="1">
-        <v>2020</v>
+      <c r="A111" t="s">
+        <v>13</v>
       </c>
       <c r="B111" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C111">
         <v>31.591292986946566</v>
@@ -2016,11 +2049,11 @@
       </c>
     </row>
     <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A112" s="1">
-        <v>2020</v>
+      <c r="A112" t="s">
+        <v>13</v>
       </c>
       <c r="B112" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C112">
         <v>36.733486231130179</v>
@@ -2030,11 +2063,11 @@
       </c>
     </row>
     <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A113" s="1">
-        <v>2020</v>
+      <c r="A113" t="s">
+        <v>13</v>
       </c>
       <c r="B113" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C113">
         <v>38.051152669653412</v>
@@ -2044,11 +2077,11 @@
       </c>
     </row>
     <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A114" s="1">
-        <v>2020</v>
+      <c r="A114" t="s">
+        <v>13</v>
       </c>
       <c r="B114" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C114">
         <v>30.023896370036081</v>
@@ -2058,11 +2091,11 @@
       </c>
     </row>
     <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A115" s="1">
-        <v>2020</v>
+      <c r="A115" t="s">
+        <v>13</v>
       </c>
       <c r="B115" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C115">
         <v>29.777461947239438</v>
@@ -2072,11 +2105,11 @@
       </c>
     </row>
     <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A116" s="1">
-        <v>2020</v>
+      <c r="A116" t="s">
+        <v>13</v>
       </c>
       <c r="B116" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C116">
         <v>30.115179339572411</v>
@@ -2086,11 +2119,11 @@
       </c>
     </row>
     <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A117" s="1">
-        <v>2020</v>
+      <c r="A117" t="s">
+        <v>13</v>
       </c>
       <c r="B117" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C117">
         <v>30.863691189496603</v>
@@ -2100,11 +2133,11 @@
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A118" s="1">
-        <v>2020</v>
+      <c r="A118" t="s">
+        <v>13</v>
       </c>
       <c r="B118" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C118">
         <v>36.400063387546297</v>
@@ -2114,25 +2147,25 @@
       </c>
     </row>
     <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A119" s="1">
-        <v>2020</v>
+      <c r="A119" t="s">
+        <v>13</v>
       </c>
       <c r="B119" t="s">
+        <v>24</v>
+      </c>
+      <c r="C119" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D119" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A120" t="s">
         <v>13</v>
       </c>
-      <c r="C119" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D119" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A120" s="1">
-        <v>2020</v>
-      </c>
       <c r="B120" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C120">
         <v>35.451150571968746</v>
@@ -2142,11 +2175,11 @@
       </c>
     </row>
     <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A121" s="1">
-        <v>2020</v>
+      <c r="A121" t="s">
+        <v>13</v>
       </c>
       <c r="B121" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C121">
         <v>39.509406302674243</v>
@@ -2156,11 +2189,11 @@
       </c>
     </row>
     <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A122" s="1">
-        <v>2021</v>
+      <c r="A122" t="s">
+        <v>14</v>
       </c>
       <c r="B122" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C122">
         <v>32.142597427901237</v>
@@ -2170,11 +2203,11 @@
       </c>
     </row>
     <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A123" s="1">
-        <v>2021</v>
+      <c r="A123" t="s">
+        <v>14</v>
       </c>
       <c r="B123" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C123">
         <v>28.529036613304051</v>
@@ -2184,11 +2217,11 @@
       </c>
     </row>
     <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A124" s="1">
-        <v>2021</v>
+      <c r="A124" t="s">
+        <v>14</v>
       </c>
       <c r="B124" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C124">
         <v>28.740144703529072</v>
@@ -2198,11 +2231,11 @@
       </c>
     </row>
     <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A125" s="1">
-        <v>2021</v>
+      <c r="A125" t="s">
+        <v>14</v>
       </c>
       <c r="B125" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C125">
         <v>33.864512066644807</v>
@@ -2212,11 +2245,11 @@
       </c>
     </row>
     <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A126" s="1">
-        <v>2021</v>
+      <c r="A126" t="s">
+        <v>14</v>
       </c>
       <c r="B126" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C126">
         <v>28.634239042099377</v>
@@ -2226,11 +2259,11 @@
       </c>
     </row>
     <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A127" s="1">
-        <v>2021</v>
+      <c r="A127" t="s">
+        <v>14</v>
       </c>
       <c r="B127" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C127">
         <v>26.355133740410956</v>
@@ -2240,11 +2273,11 @@
       </c>
     </row>
     <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A128" s="1">
-        <v>2021</v>
+      <c r="A128" t="s">
+        <v>14</v>
       </c>
       <c r="B128" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C128">
         <v>19.206398119252874</v>
@@ -2254,11 +2287,11 @@
       </c>
     </row>
     <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A129" s="1">
-        <v>2021</v>
+      <c r="A129" t="s">
+        <v>14</v>
       </c>
       <c r="B129" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C129">
         <v>17.204920088467741</v>
@@ -2268,11 +2301,11 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A130" s="1">
-        <v>2021</v>
+      <c r="A130" t="s">
+        <v>14</v>
       </c>
       <c r="B130" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C130">
         <v>29.177165687407406</v>
@@ -2282,11 +2315,11 @@
       </c>
     </row>
     <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A131" s="1">
-        <v>2021</v>
+      <c r="A131" t="s">
+        <v>14</v>
       </c>
       <c r="B131" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C131">
         <v>29.202242642416667</v>
@@ -2296,11 +2329,11 @@
       </c>
     </row>
     <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A132" s="1">
-        <v>2021</v>
+      <c r="A132" t="s">
+        <v>14</v>
       </c>
       <c r="B132" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C132">
         <v>30.356772037416665</v>
@@ -2310,11 +2343,11 @@
       </c>
     </row>
     <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A133" s="1">
-        <v>2021</v>
+      <c r="A133" t="s">
+        <v>14</v>
       </c>
       <c r="B133" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C133">
         <v>31.998705114333333</v>
@@ -2336,11 +2369,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED7C510-0EA0-497B-B15B-009BEC254858}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E808599A-4BEE-4CDE-9BA4-6DB348F1246D}">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2350,20 +2383,20 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>2011</v>
       </c>
       <c r="B2">
@@ -2381,25 +2414,25 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>2012</v>
       </c>
       <c r="B3">
         <v>1.400532786885246</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
       </c>
       <c r="E3">
-        <f>AVERAGE(B3:D3)</f>
-        <v>0.46684426229508197</v>
+        <f t="shared" ref="E3:E12" si="0">AVERAGE(B3:D3)</f>
+        <v>1.400532786885246</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>2013</v>
       </c>
       <c r="B4">
@@ -2408,16 +2441,16 @@
       <c r="C4">
         <v>5.6309756097560975</v>
       </c>
-      <c r="D4">
-        <v>0</v>
+      <c r="D4" t="s">
+        <v>31</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E12" si="0">AVERAGE(B4:D4)</f>
-        <v>3.798425978445831</v>
+        <f t="shared" si="0"/>
+        <v>5.6976389676687464</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>2014</v>
       </c>
       <c r="B5">
@@ -2435,7 +2468,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>2015</v>
       </c>
       <c r="B6">
@@ -2453,7 +2486,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>2016</v>
       </c>
       <c r="B7">
@@ -2471,7 +2504,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>2017</v>
       </c>
       <c r="B8">
@@ -2481,7 +2514,7 @@
         <v>2.986470588235294</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
@@ -2489,7 +2522,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>2018</v>
       </c>
       <c r="B9">
@@ -2507,7 +2540,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>2019</v>
       </c>
       <c r="B10">
@@ -2525,7 +2558,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>2020</v>
       </c>
       <c r="B11">
@@ -2543,7 +2576,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>2021</v>
       </c>
       <c r="B12">
@@ -2563,7 +2596,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E2 E3:E12" formulaRange="1"/>
+    <ignoredError sqref="E2 E5:E12" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>